<commit_message>
Correção de alguns modelos
</commit_message>
<xml_diff>
--- a/Modelos UML/Descrição UseCases/ComprarCarro.xlsx
+++ b/Modelos UML/Descrição UseCases/ComprarCarro.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Actor input</t>
   </si>
@@ -66,40 +66,43 @@
     <t>2. Indica que quer comprar carro</t>
   </si>
   <si>
-    <t>6. Pergunta qual a forma de personalizar o carro</t>
-  </si>
-  <si>
-    <t>7. Escolhe configuração ótima</t>
-  </si>
-  <si>
-    <t>8.&lt;&lt;include&gt;&gt; Escolher configuração ótima</t>
-  </si>
-  <si>
-    <t>Alternativa 1 [Escolher Pacote] (passo 7)</t>
-  </si>
-  <si>
-    <t>7.1 Escolhe Pacote</t>
-  </si>
-  <si>
-    <t>7.2 &lt;&lt;include&gt;&gt; Escolhe Pacote</t>
-  </si>
-  <si>
-    <t>Alternativa 2 [Escolher Especificações] (passo 7)</t>
-  </si>
-  <si>
-    <t>7.1 Escolhe Especificações</t>
-  </si>
-  <si>
-    <t>7.2 &lt;&lt;include&gt;&gt; Escolher Especificações</t>
-  </si>
-  <si>
     <t>5. Seleciona modelo que pretende comprar</t>
   </si>
   <si>
     <t>4. Mostra todos os modelos disponiveis</t>
   </si>
   <si>
-    <t>3. Verifica modelos disponiveis</t>
+    <t>3. Obtém modelos disponiveis</t>
+  </si>
+  <si>
+    <t>6. Regista modelo escolhido</t>
+  </si>
+  <si>
+    <t>7. Pergunta qual a forma de personalizar o carro</t>
+  </si>
+  <si>
+    <t>9.&lt;&lt;include&gt;&gt; Escolher configuração ótima</t>
+  </si>
+  <si>
+    <t>8. Escolhe configuração ótima</t>
+  </si>
+  <si>
+    <t>Alternativa 1 [Escolher Pacote] (passo 8)</t>
+  </si>
+  <si>
+    <t>Alternativa 2 [Escolher Especificações] (passo 8)</t>
+  </si>
+  <si>
+    <t>8.1 Escolhe Pacote</t>
+  </si>
+  <si>
+    <t>8.2 &lt;&lt;include&gt;&gt; Escolhe Pacote</t>
+  </si>
+  <si>
+    <t>8.2 &lt;&lt;include&gt;&gt; Escolher Especificações</t>
+  </si>
+  <si>
+    <t>8.1 Escolhe Especificações</t>
   </si>
 </sst>
 </file>
@@ -693,10 +696,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D20"/>
+  <dimension ref="B1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -773,20 +776,20 @@
       <c r="B9" s="22"/>
       <c r="C9" s="5"/>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="22"/>
       <c r="C10" s="5"/>
       <c r="D10" s="1" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="22"/>
       <c r="C11" s="5" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -794,74 +797,81 @@
       <c r="B12" s="22"/>
       <c r="C12" s="5"/>
       <c r="D12" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="22"/>
-      <c r="C13" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="1"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="22"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="C14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="2"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="B16" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="16"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="3"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="10"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="16"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="14" t="s">
+      <c r="B19" s="16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="10"/>
+    </row>
+    <row r="20" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="16"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="16"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B16:B18"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="B6:B14"/>
+    <mergeCell ref="B6:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>